<commit_message>
New Cad: Motor Mount
</commit_message>
<xml_diff>
--- a/airframe weight calculations.xlsx
+++ b/airframe weight calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/jamesdrosdick_vt_edu/Documents/school/Team_45_FFUAV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive - Virginia Tech\Documents\GitHub\Team_45_FFUAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41FF7EBC-D0CA-48EC-B603-600458A9A5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF9F6E3-E989-4AC9-BD0C-85DE5DE92DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">thickness </t>
   </si>
   <si>
-    <t>Hub</t>
-  </si>
-  <si>
     <t>S (mm)</t>
   </si>
   <si>
@@ -111,12 +108,15 @@
   </si>
   <si>
     <t>motor mounts</t>
+  </si>
+  <si>
+    <t>Hub (hexagon)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,24 +470,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,15 +496,15 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -521,17 +521,17 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="M4" s="1">
         <f>SUM(M5:M12)</f>
         <v>10078.03721112038</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -558,14 +558,14 @@
         <v>723.38826484656533</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5">
         <f>G5*8</f>
         <v>5787.1061187725227</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -581,8 +581,8 @@
         <v>940</v>
       </c>
       <c r="E6">
-        <f>B6-C6</f>
-        <v>6.3500000000000014</v>
+        <f>(B6-C6)/2</f>
+        <v>3.1750000000000007</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
@@ -592,38 +592,38 @@
         <v>2863.7310923478558</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <f>B16*8</f>
         <v>960</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M8">
         <f>B19*8</f>
         <v>467.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
       </c>
       <c r="B10">
         <v>191.34</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -631,48 +631,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <f>(B10^2) * (1 + SQRT(2))*2*B11</f>
         <v>530320.57265701029</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <f>B1*B12</f>
         <v>1431.8655461739279</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
       </c>
       <c r="B16">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
       </c>
       <c r="B19">
         <v>58.4</v>

</xml_diff>

<commit_message>
james dump- dxf files for cnc clamps
</commit_message>
<xml_diff>
--- a/airframe weight calculations.xlsx
+++ b/airframe weight calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\OneDrive - Virginia Tech\Documents\GitHub\Team_45_FFUAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF9F6E3-E989-4AC9-BD0C-85DE5DE92DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31C2142-012D-420C-8C05-39578A28A9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">desity </t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Hub (hexagon)</t>
+  </si>
+  <si>
+    <t>plate</t>
+  </si>
+  <si>
+    <t>clamp</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,7 +534,7 @@
       </c>
       <c r="M4" s="1">
         <f>SUM(M5:M12)</f>
-        <v>10078.03721112038</v>
+        <v>8573.839038213393</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -539,7 +545,7 @@
         <v>1.25</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>1.0840000000000001</v>
       </c>
       <c r="D5">
         <f>D6/25.4</f>
@@ -547,22 +553,22 @@
       </c>
       <c r="E5">
         <f>B5-C5</f>
-        <v>0.25</v>
+        <v>0.16599999999999993</v>
       </c>
       <c r="F5">
         <f>PI()*((B6/2)^2 - (C6/2)^2)*D6</f>
-        <v>267921.57957280194</v>
+        <v>184541.52617956384</v>
       </c>
       <c r="G5">
         <f>F5*B1</f>
-        <v>723.38826484656533</v>
+        <v>498.26212068482238</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
       </c>
       <c r="M5">
         <f>G5*8</f>
-        <v>5787.1061187725227</v>
+        <v>3986.096965478579</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -575,21 +581,21 @@
       </c>
       <c r="C6">
         <f>C5*25.4</f>
-        <v>25.4</v>
+        <v>27.5336</v>
       </c>
       <c r="D6">
         <v>940</v>
       </c>
       <c r="E6">
         <f>(B6-C6)/2</f>
-        <v>3.1750000000000007</v>
+        <v>2.1082000000000001</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
       </c>
       <c r="M6">
         <f>B13*2</f>
-        <v>2863.7310923478558</v>
+        <v>3030.7820727348139</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -606,8 +612,8 @@
         <v>23</v>
       </c>
       <c r="M8">
-        <f>B19*8</f>
-        <v>467.2</v>
+        <f>B22*8</f>
+        <v>596.96</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -628,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>3.1749999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -637,7 +643,7 @@
       </c>
       <c r="B12">
         <f>(B10^2) * (1 + SQRT(2))*2*B11</f>
-        <v>530320.57265701029</v>
+        <v>561255.93939533585</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -646,7 +652,7 @@
       </c>
       <c r="B13">
         <f>B1*B12</f>
-        <v>1431.8655461739279</v>
+        <v>1515.391036367407</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -665,17 +671,55 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19">
         <v>58.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>257</v>
+      </c>
+      <c r="L20">
+        <f>24*48 - 257*2 - 42.5*60*8</f>
+        <v>-19762</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>55.62</v>
+      </c>
+      <c r="J21">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f>SUM(B20:B21)</f>
+        <v>74.62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <f>609.6 * 609.6*2 - 165806*2 - 42.5*60*8</f>
+        <v>391212.32000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>